<commit_message>
Updates to Case study code
Case study 2 code updates to promote a clean and auditable script. Case study 3 added to the project folder.
</commit_message>
<xml_diff>
--- a/CaseStudy2_Wang2024/res/feature importance.xlsx
+++ b/CaseStudy2_Wang2024/res/feature importance.xlsx
@@ -448,31 +448,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TM/YB</t>
+          <t>YB/LU</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>166.6</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ER/TM</t>
+          <t>TM/YB</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>163.4</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>YB/LU</t>
+          <t>TH/U</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>162.4</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>155.2</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="6">
@@ -492,17 +492,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>145</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Y/LA/TB</t>
+          <t>ER/TM</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>141.4</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="8">
@@ -512,87 +512,87 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>128</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EU/GD</t>
+          <t>Y/LA/TB</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>123.6</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TH/U</t>
+          <t>EU/GD</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>123.4</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HO-LU</t>
+          <t>Y/CE*/TH</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>120.6</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NB/LA/CE*</t>
+          <t>TA/U</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>120</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TA/U</t>
+          <t>HF-U</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>118.2</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Y/CE*/TH</t>
+          <t>LU/TH</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>118.2</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>LU/TH</t>
+          <t>HO-LU</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>117.8</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PR/ND/EU*</t>
+          <t>EU**EU**TA</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>117</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="17">
@@ -602,17 +602,17 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>116.2</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PR/ND/TA</t>
+          <t>CE/GD</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>113.8</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="19">
@@ -622,1017 +622,1017 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>113.4</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CE/HF/TH</t>
+          <t>Y/YB/TH</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>113.2</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Y/YB/TH</t>
+          <t>NB/LA/CE*</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>111.4</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Y/CE*/EU</t>
+          <t>CE/HF/TH</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>111.4</v>
+        <v>995.9999999999997</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CE/U</t>
+          <t>TI*Y*EU*</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>110.2</v>
+        <v>985.9999999999998</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>NB/LU/TA</t>
+          <t>CE/TA/U</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>110</v>
+        <v>983.9999999999998</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>EU**EU**TA</t>
+          <t>PR/EU/TA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>109.2</v>
+        <v>981.9999999999998</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Y/CE/EU*</t>
+          <t>CE/U</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>106.4</v>
+        <v>976.0000000000002</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>HF-U</t>
+          <t>PR/ND/EU*</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>105</v>
+        <v>957.9999999999998</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>EU**HF*TA</t>
+          <t>CE-ND-TA</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>104.2</v>
+        <v>945.9999999999994</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TH-U</t>
+          <t>Y/CE*/EU</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>103.4</v>
+        <v>942.0000000000003</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>TI/HF/HF</t>
+          <t>Y/CE/EU*</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>101.4</v>
+        <v>939.9999999999997</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SM/GD</t>
+          <t>Y/DY/HF</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>101.4</v>
+        <v>936.0000000000001</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TI*Y*EU*</t>
+          <t>CE/DY/U</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>101.2</v>
+        <v>929.9999999999995</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CE/EU*/TH</t>
+          <t>TI/HF/HF</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>100.6</v>
+        <v>926.0000000000002</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CE/DY/U</t>
+          <t>NB/LU/TA</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>100.4</v>
+        <v>925.9999999999997</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TI/NB/EU*</t>
+          <t>TH-U</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>99.59999999999999</v>
+        <v>920</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GD/TB</t>
+          <t>CE/EU*/TH</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>99</v>
+        <v>910</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CE-ND-TA</t>
+          <t>TI*EU*HF</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>99</v>
+        <v>899.9999999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Y/DY/HF</t>
+          <t>NB/CE/CE</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>97</v>
+        <v>897.9999999999998</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TI*EU**U</t>
+          <t>TI*TI*U</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>96.40000000000001</v>
+        <v>894.0000000000005</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>TI*TI*U</t>
+          <t>EU**HF*TA</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>96.40000000000001</v>
+        <v>892.0000000000002</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PR/EU/TA</t>
+          <t>TI/NB/EU*</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>95.19999999999999</v>
+        <v>885.9999999999999</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TI*EU*HF</t>
+          <t>YB/LU/TA</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>94.40000000000001</v>
+        <v>881.9999999999995</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TI*Y*TA</t>
+          <t>PR/ND/TA</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>93.99999999999999</v>
+        <v>878.0000000000001</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CE/TA/U</t>
+          <t>CE/EU*/EU*</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>93.80000000000001</v>
+        <v>866</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CE/GD</t>
+          <t>TI/EU*/HF</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>93.19999999999999</v>
+        <v>854</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>CE/EU*/EU*</t>
+          <t>Y/NB</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>92.59999999999999</v>
+        <v>852.0000000000001</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>HF-TH-U</t>
+          <t>TI*TI*CE</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>91.59999999999999</v>
+        <v>840.0000000000005</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>NB/CE/CE</t>
+          <t>ER/TM/HF</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>90.59999999999999</v>
+        <v>837.9999999999999</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>LA+EU*+TA</t>
+          <t>TI*NB*TA</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>90.39999999999999</v>
+        <v>834</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Y/CE/U</t>
+          <t>TI*TI*TA</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>89.80000000000001</v>
+        <v>824</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>TI*TI*CE</t>
+          <t>TI*Y*TA</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>89.40000000000001</v>
+        <v>818.0000000000003</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>YB/LU/TA</t>
+          <t>Y/NB/ER</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>89.40000000000001</v>
+        <v>817.9999999999999</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ER/TM/HF</t>
+          <t>HF-TH-U</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>89</v>
+        <v>816.0000000000001</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TI/EU*/HF</t>
+          <t>TI*HF*TA</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>88.8</v>
+        <v>814.0000000000003</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Y*CE*EU*</t>
+          <t>GD/TB</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>87</v>
+        <v>807.9999999999999</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>EU**HF*HF</t>
+          <t>CE/EU*</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>86.40000000000001</v>
+        <v>806</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CE/GD/HF</t>
+          <t>EU**HF*HF</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>86.19999999999999</v>
+        <v>805.9999999999998</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>TI*NB*TA</t>
+          <t>Y/CE/U</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>85.8</v>
+        <v>800</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>SM/EU/TA</t>
+          <t>Y*CE*EU*</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>84.8</v>
+        <v>798.0000000000005</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>CE/DY/DY</t>
+          <t>CE/EU/TH</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>83.8</v>
+        <v>792.0000000000001</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Y/NB/ER</t>
+          <t>DY-LU-LU</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>83.40000000000001</v>
+        <v>787.9999999999995</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ER/YB/HF</t>
+          <t>ER-LU-LU</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>83.2</v>
+        <v>784.0000000000003</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>DY/LU</t>
+          <t>CE/DY/DY</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>83</v>
+        <v>784</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>HO-LU-TA</t>
+          <t>SM/EU/TA</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>83</v>
+        <v>783.9999999999999</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>CE/EU/TA</t>
+          <t>ER/YB/HF</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>83</v>
+        <v>780</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ER-LU-LU</t>
+          <t>TI*EU**U</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>82.59999999999999</v>
+        <v>778</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CE*EU**HF</t>
+          <t>SM/GD</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>82.59999999999999</v>
+        <v>756.0000000000001</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>EU*/TA/TA</t>
+          <t>LA+EU*+TA</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>82.40000000000001</v>
+        <v>740.0000000000001</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Y/NB</t>
+          <t>CE*EU**HF</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>81.59999999999999</v>
+        <v>736.0000000000002</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>DY-LU-LU</t>
+          <t>ND-EU-EU*</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>81.40000000000001</v>
+        <v>731.9999999999998</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>CE/EU*</t>
+          <t>CE/GD/HF</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>81</v>
+        <v>731.9999999999995</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>EU/GD/HF</t>
+          <t>CE**ND*HF</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>80.80000000000001</v>
+        <v>727.9999999999999</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ND-EU-EU*</t>
+          <t>ER/LU</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>80.59999999999999</v>
+        <v>723.9999999999999</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Y/HO</t>
+          <t>DY/LU</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>80.40000000000001</v>
+        <v>722.0000000000001</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Y/NB/CE</t>
+          <t>CE/TH</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>80.40000000000001</v>
+        <v>718.0000000000001</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ER/LU</t>
+          <t>NB*EU**U</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>80</v>
+        <v>715.9999999999999</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Y*EU**HF</t>
+          <t>NB/HF/U</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>80</v>
+        <v>708.0000000000002</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>TI*HF*HF</t>
+          <t>EU/GD/HF</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>79.59999999999999</v>
+        <v>707.9999999999997</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Y/ER</t>
+          <t>EU*/TA/TA</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>79</v>
+        <v>701.9999999999998</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>TI/EU*/TA</t>
+          <t>Y/HO</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>78.8</v>
+        <v>699.9999999999995</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>CE/TH</t>
+          <t>Y/EU*/U</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>78.59999999999999</v>
+        <v>698.0000000000002</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>TI*TI*TA</t>
+          <t>TM/YB/HF</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>77.59999999999999</v>
+        <v>695.9999999999995</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Y/TM</t>
+          <t>HO/TM</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>77.39999999999999</v>
+        <v>691.9999999999995</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>NB/HF/U</t>
+          <t>Y/TM</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>77.2</v>
+        <v>688</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>CE**ND*HF</t>
+          <t>CE/EU*/U</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>76.59999999999999</v>
+        <v>686</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>CE/EU/TH</t>
+          <t>NB/HF/TH</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>75.59999999999999</v>
+        <v>685.9999999999999</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>TM/YB/HF</t>
+          <t>CE/TA/TH</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>75.40000000000001</v>
+        <v>676.0000000000002</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>TM/LU</t>
+          <t>TI/EU*/TA</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>73.8</v>
+        <v>676.0000000000001</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>HO/ER</t>
+          <t>Y/ER</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>72.60000000000001</v>
+        <v>670</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>TI*HF*TA</t>
+          <t>HO-LU-TA</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>72.59999999999999</v>
+        <v>662</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Y/NB/YB</t>
+          <t>TI*HF*HF</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>72.59999999999999</v>
+        <v>660</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>NB*EU**U</t>
+          <t>EU/EU*/GD</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>72.2</v>
+        <v>656.0000000000001</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>HO/TM</t>
+          <t>Y*HF*TA</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>72</v>
+        <v>650.0000000000002</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>CE/TA/TH</t>
+          <t>HO/ER</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>71.8</v>
+        <v>648.0000000000001</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>NB/HF/TH</t>
+          <t>Y/NB/YB</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>71.59999999999999</v>
+        <v>634.0000000000001</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>DY-LU-TA</t>
+          <t>TI/HF</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>70</v>
+        <v>632.0000000000002</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>SM/GD/HF</t>
+          <t>Y/SM</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>69.80000000000001</v>
+        <v>630</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>CE/SM/HF</t>
+          <t>CE/HF/HF</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>69.59999999999999</v>
+        <v>628.0000000000002</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>CE/EU*/U</t>
+          <t>NB-TA-TA</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>68.40000000000001</v>
+        <v>624.0000000000001</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>EU/EU*/GD</t>
+          <t>SM/GD/HF</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>68.19999999999999</v>
+        <v>622.0000000000002</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Y/EU*/U</t>
+          <t>CE/SM/HF</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>67.8</v>
+        <v>621.9999999999999</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>NB/TH/U</t>
+          <t>Y/NB/EU*</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>67.40000000000001</v>
+        <v>611.9999999999999</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>TI*TI*DY</t>
+          <t>CE/EU/EU*</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>67.40000000000001</v>
+        <v>610.0000000000001</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Y/SM</t>
+          <t>Y/YB</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>67</v>
+        <v>603.9999999999998</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>CE/HF/HF</t>
+          <t>TM/LU</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>66.59999999999999</v>
+        <v>601.9999999999999</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>ND-EU-EU</t>
+          <t>NB/TH/U</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>66.40000000000001</v>
+        <v>599.9999999999999</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Y/NB/EU*</t>
+          <t>Y/NB/CE</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>65.8</v>
+        <v>597.9999999999999</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Y*HF*TA</t>
+          <t>CE/EU/TA</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>65.40000000000001</v>
+        <v>586</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>CE/EU/EU*</t>
+          <t>DY-LU-TA</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>64.60000000000001</v>
+        <v>584.0000000000001</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Y/DY</t>
+          <t>TI*TI*DY</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>64.40000000000001</v>
+        <v>580.0000000000002</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Y/YB</t>
+          <t>Y*EU**HF</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>62</v>
+        <v>572</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>CE/EU/HF</t>
+          <t>Y/DY</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>60.8</v>
+        <v>571.9999999999998</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>TB/DY/HF</t>
+          <t>Y/TH</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>60</v>
+        <v>566.0000000000003</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Y/DY/TA</t>
+          <t>ND-EU-EU</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>59.2</v>
+        <v>564</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Y/TH</t>
+          <t>CE/EU/HF</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>57.8</v>
+        <v>540.0000000000002</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>TI/HF</t>
+          <t>TB/DY/HF</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>53.59999999999999</v>
+        <v>534.0000000000001</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>NB/HF/TA</t>
+          <t>Y/DY/TA</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>52.6</v>
+        <v>531.9999999999998</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>NB-TA-TA</t>
+          <t>TB/LU/HF</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>52.4</v>
+        <v>432.0000000000001</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>TA*U</t>
+          <t>NB/HF/TA</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>52.2</v>
+        <v>425.9999999999999</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>TB/LU/HF</t>
+          <t>TA*U</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>42.2</v>
+        <v>414.0000000000001</v>
       </c>
     </row>
     <row r="121">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>30.8</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Case Study 3
Major updates to code of case study 3. Minor updates to Case Study 1 and 2, particularly for population comparisons.
</commit_message>
<xml_diff>
--- a/CaseStudy2_Wang2024/res/feature importance.xlsx
+++ b/CaseStudy2_Wang2024/res/feature importance.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1572</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="3">
@@ -462,17 +462,17 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1462</v>
+        <v>2218.200000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TH/U</t>
+          <t>ER/TM</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1408</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1360</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="6">
@@ -492,17 +492,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1360</v>
+        <v>1854.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ER/TM</t>
+          <t>Y/LA/TB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1348</v>
+        <v>1840.799999999999</v>
       </c>
     </row>
     <row r="8">
@@ -512,17 +512,17 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1298</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Y/LA/TB</t>
+          <t>TH/U</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1282</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1248</v>
+        <v>1698.2</v>
       </c>
     </row>
     <row r="11">
@@ -542,397 +542,397 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1156</v>
+        <v>1642.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>TA/U</t>
+          <t>YB/LU/HF</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1148</v>
+        <v>1621.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HF-U</t>
+          <t>TA/U</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1120</v>
+        <v>1615.6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LU/TH</t>
+          <t>HO-LU</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1098</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HO-LU</t>
+          <t>NB/LA/CE*</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1090</v>
+        <v>1581.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EU**EU**TA</t>
+          <t>ER/YB</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1072</v>
+        <v>1577.2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>YB/LU/HF</t>
+          <t>PR/ND/EU*</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1052</v>
+        <v>1535.599999999999</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CE/GD</t>
+          <t>LU/TH</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1050</v>
+        <v>1517.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ER/YB</t>
+          <t>EU**EU**TA</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1040</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Y/YB/TH</t>
+          <t>Y/CE*/EU</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1006</v>
+        <v>1451.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NB/LA/CE*</t>
+          <t>TI*Y*EU*</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1000</v>
+        <v>1444.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CE/HF/TH</t>
+          <t>NB/LU/TA</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>995.9999999999997</v>
+        <v>1426.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TI*Y*EU*</t>
+          <t>GD/TB</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>985.9999999999998</v>
+        <v>1423.4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CE/TA/U</t>
+          <t>Y/YB/TH</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>983.9999999999998</v>
+        <v>1421.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PR/EU/TA</t>
+          <t>PR/ND/TA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>981.9999999999998</v>
+        <v>1396.2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CE/U</t>
+          <t>Y/CE/EU*</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>976.0000000000002</v>
+        <v>1390.2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>PR/ND/EU*</t>
+          <t>CE/HF/TH</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>957.9999999999998</v>
+        <v>1389.4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CE-ND-TA</t>
+          <t>HF-U</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>945.9999999999994</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Y/CE*/EU</t>
+          <t>TH-U</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>942.0000000000003</v>
+        <v>1377.6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Y/CE/EU*</t>
+          <t>CE/U</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>939.9999999999997</v>
+        <v>1360.8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Y/DY/HF</t>
+          <t>CE/EU*/EU*</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>936.0000000000001</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CE/DY/U</t>
+          <t>CE/EU*/TH</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>929.9999999999995</v>
+        <v>1345.2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TI/HF/HF</t>
+          <t>Y/DY/HF</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>926.0000000000002</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>NB/LU/TA</t>
+          <t>CE-ND-TA</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>925.9999999999997</v>
+        <v>1341.4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TH-U</t>
+          <t>EU**HF*TA</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>920</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CE/EU*/TH</t>
+          <t>YB/LU/TA</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>910</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TI*EU*HF</t>
+          <t>CE/DY/U</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>899.9999999999999</v>
+        <v>1310.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>NB/CE/CE</t>
+          <t>PR/EU/TA</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>897.9999999999998</v>
+        <v>1304.2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TI*TI*U</t>
+          <t>TI/NB/EU*</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>894.0000000000005</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>EU**HF*TA</t>
+          <t>TI*EU**U</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>892.0000000000002</v>
+        <v>1299.2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TI/NB/EU*</t>
+          <t>TI*TI*U</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>885.9999999999999</v>
+        <v>1297.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>YB/LU/TA</t>
+          <t>ER/TM/HF</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>881.9999999999995</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>PR/ND/TA</t>
+          <t>CE/GD</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>878.0000000000001</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CE/EU*/EU*</t>
+          <t>TI/HF/HF</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>866</v>
+        <v>1285.8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>TI/EU*/HF</t>
+          <t>HF-TH-U</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>854</v>
+        <v>1280.8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Y/NB</t>
+          <t>NB/CE/CE</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>852.0000000000001</v>
+        <v>1271.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>TI*TI*CE</t>
+          <t>CE/TA/U</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>840.0000000000005</v>
+        <v>1268.000000000001</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ER/TM/HF</t>
+          <t>TI/EU*/HF</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>837.9999999999999</v>
+        <v>1259.2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>TI*NB*TA</t>
+          <t>Y/CE/U</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>834</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>TI*TI*TA</t>
+          <t>TI*EU*HF</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>824</v>
+        <v>1247.8</v>
       </c>
     </row>
     <row r="51">
@@ -942,207 +942,207 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>818.0000000000003</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Y/NB/ER</t>
+          <t>SM/GD</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>817.9999999999999</v>
+        <v>1220.8</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>HF-TH-U</t>
+          <t>EU**HF*HF</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>816.0000000000001</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TI*HF*TA</t>
+          <t>TI*TI*CE</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>814.0000000000003</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>GD/TB</t>
+          <t>Y*CE*EU*</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>807.9999999999999</v>
+        <v>1177.2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CE/EU*</t>
+          <t>LA+EU*+TA</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>806</v>
+        <v>1171.6</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>EU**HF*HF</t>
+          <t>ND-EU-EU*</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>805.9999999999998</v>
+        <v>1161.8</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Y/CE/U</t>
+          <t>CE/EU*</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>800</v>
+        <v>1157.6</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Y*CE*EU*</t>
+          <t>ER-LU-LU</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>798.0000000000005</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>CE/EU/TH</t>
+          <t>TI*NB*TA</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>792.0000000000001</v>
+        <v>1154.8</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>DY-LU-LU</t>
+          <t>ER/YB/HF</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>787.9999999999995</v>
+        <v>1152.2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>ER-LU-LU</t>
+          <t>DY-LU-LU</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>784.0000000000003</v>
+        <v>1144.6</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>CE/DY/DY</t>
+          <t>Y/ER</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>784</v>
+        <v>1133.2</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SM/EU/TA</t>
+          <t>CE/GD/HF</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>783.9999999999999</v>
+        <v>1114.2</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ER/YB/HF</t>
+          <t>SM/EU/TA</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>780</v>
+        <v>1105.4</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>TI*EU**U</t>
+          <t>CE*EU**HF</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>778</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SM/GD</t>
+          <t>Y/HO</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>756.0000000000001</v>
+        <v>1100.8</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>LA+EU*+TA</t>
+          <t>HO-LU-TA</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>740.0000000000001</v>
+        <v>1096.2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>CE*EU**HF</t>
+          <t>Y/NB</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>736.0000000000002</v>
+        <v>1091.2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ND-EU-EU*</t>
+          <t>ER/LU</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>731.9999999999998</v>
+        <v>1090.6</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>CE/GD/HF</t>
+          <t>TI*TI*TA</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>731.9999999999995</v>
+        <v>1085.4</v>
       </c>
     </row>
     <row r="72">
@@ -1152,487 +1152,487 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>727.9999999999999</v>
+        <v>1081.8</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>ER/LU</t>
+          <t>Y/NB/ER</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>723.9999999999999</v>
+        <v>1078.6</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>DY/LU</t>
+          <t>EU/GD/HF</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>722.0000000000001</v>
+        <v>1076.6</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>CE/TH</t>
+          <t>DY/LU</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>718.0000000000001</v>
+        <v>1074.4</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>NB*EU**U</t>
+          <t>CE/EU/TH</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>715.9999999999999</v>
+        <v>1071.4</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>NB/HF/U</t>
+          <t>TI*HF*TA</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>708.0000000000002</v>
+        <v>1066.2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>EU/GD/HF</t>
+          <t>CE/DY/DY</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>707.9999999999997</v>
+        <v>1061.8</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>EU*/TA/TA</t>
+          <t>HO/TM</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>701.9999999999998</v>
+        <v>1053.4</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Y/HO</t>
+          <t>HO/ER</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>699.9999999999995</v>
+        <v>1048.799999999999</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Y/EU*/U</t>
+          <t>TM/YB/HF</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>698.0000000000002</v>
+        <v>1047.8</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>TM/YB/HF</t>
+          <t>TI*HF*HF</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>695.9999999999995</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>HO/TM</t>
+          <t>NB/HF/TH</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>691.9999999999995</v>
+        <v>1031.8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Y/TM</t>
+          <t>TM/LU</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>688</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>CE/EU*/U</t>
+          <t>Y/TM</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>686</v>
+        <v>1027.6</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>NB/HF/TH</t>
+          <t>TI/EU*/TA</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>685.9999999999999</v>
+        <v>1025.4</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>CE/TA/TH</t>
+          <t>NB*EU**U</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>676.0000000000002</v>
+        <v>1023.6</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>TI/EU*/TA</t>
+          <t>CE/EU/EU*</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>676.0000000000001</v>
+        <v>1011.6</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Y/ER</t>
+          <t>CE/TH</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>670</v>
+        <v>1010.4</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>HO-LU-TA</t>
+          <t>CE/EU/TA</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>662</v>
+        <v>1001.8</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>TI*HF*HF</t>
+          <t>NB/HF/U</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>660</v>
+        <v>999.6</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>EU/EU*/GD</t>
+          <t>EU*/TA/TA</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>656.0000000000001</v>
+        <v>992.2</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Y*HF*TA</t>
+          <t>CE/TA/TH</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>650.0000000000002</v>
+        <v>985.1999999999999</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>HO/ER</t>
+          <t>CE/HF/HF</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>648.0000000000001</v>
+        <v>975.2</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Y/NB/YB</t>
+          <t>Y/EU*/U</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>634.0000000000001</v>
+        <v>972.6</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>TI/HF</t>
+          <t>EU/EU*/GD</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>632.0000000000002</v>
+        <v>969.9999999999999</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Y/SM</t>
+          <t>TI*TI*DY</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>630</v>
+        <v>939.7999999999998</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>CE/HF/HF</t>
+          <t>Y/NB/EU*</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>628.0000000000002</v>
+        <v>936.6000000000003</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>NB-TA-TA</t>
+          <t>Y/SM</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>624.0000000000001</v>
+        <v>935.2000000000002</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>SM/GD/HF</t>
+          <t>CE/EU*/U</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>622.0000000000002</v>
+        <v>934.6000000000001</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>CE/SM/HF</t>
+          <t>Y/NB/YB</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>621.9999999999999</v>
+        <v>931.8000000000001</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Y/NB/EU*</t>
+          <t>Y/TH</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>611.9999999999999</v>
+        <v>930.7999999999996</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>CE/EU/EU*</t>
+          <t>Y*EU**HF</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>610.0000000000001</v>
+        <v>925.2000000000004</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Y/YB</t>
+          <t>CE/SM/HF</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>603.9999999999998</v>
+        <v>924.6</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>TM/LU</t>
+          <t>DY-LU-TA</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>601.9999999999999</v>
+        <v>923</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>NB/TH/U</t>
+          <t>ND-EU-EU</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>599.9999999999999</v>
+        <v>905.7999999999998</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Y/NB/CE</t>
+          <t>SM/GD/HF</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>597.9999999999999</v>
+        <v>898.6</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>CE/EU/TA</t>
+          <t>Y/NB/CE</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>586</v>
+        <v>897.8000000000002</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>DY-LU-TA</t>
+          <t>NB/TH/U</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>584.0000000000001</v>
+        <v>892.9999999999997</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>TI*TI*DY</t>
+          <t>Y*HF*TA</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>580.0000000000002</v>
+        <v>884.1999999999999</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Y*EU**HF</t>
+          <t>Y/YB</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>572</v>
+        <v>883.1999999999998</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Y/DY</t>
+          <t>TB/DY/HF</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>571.9999999999998</v>
+        <v>849.9999999999998</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Y/TH</t>
+          <t>TI/HF</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>566.0000000000003</v>
+        <v>843.6000000000001</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>ND-EU-EU</t>
+          <t>Y/DY</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>564</v>
+        <v>838</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>CE/EU/HF</t>
+          <t>Y/DY/TA</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>540.0000000000002</v>
+        <v>829.8000000000002</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>TB/DY/HF</t>
+          <t>CE/EU/HF</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>534.0000000000001</v>
+        <v>820.9999999999999</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Y/DY/TA</t>
+          <t>NB-TA-TA</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>531.9999999999998</v>
+        <v>772.3999999999997</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>TB/LU/HF</t>
+          <t>NB/HF/TA</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>432.0000000000001</v>
+        <v>702.8</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>NB/HF/TA</t>
+          <t>TA*U</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>425.9999999999999</v>
+        <v>633.2000000000002</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>TA*U</t>
+          <t>TB/LU/HF</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>414.0000000000001</v>
+        <v>571.3999999999999</v>
       </c>
     </row>
     <row r="121">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>334</v>
+        <v>511.9999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>